<commit_message>
Created .tex files for each filter table
</commit_message>
<xml_diff>
--- a/lab5/Band_Pass_Filter.xlsx
+++ b/lab5/Band_Pass_Filter.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ENGR202\ENGR202LAB\lab5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="21330" windowHeight="4605" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -22,75 +26,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t xml:space="preserve">VIN (V)</t>
+    <t>VIN (V)</t>
   </si>
   <si>
-    <t xml:space="preserve">Freq (Hz)</t>
+    <t>Freq (Hz)</t>
   </si>
   <si>
-    <t xml:space="preserve">VOUT(V)</t>
+    <t>VOUT(V)</t>
   </si>
   <si>
-    <t xml:space="preserve">Period (sec)</t>
+    <t>Period (sec)</t>
   </si>
   <si>
-    <t xml:space="preserve">Time Shift</t>
+    <t>Time Shift</t>
   </si>
   <si>
-    <t xml:space="preserve">Phase Shift (degree)</t>
+    <t>Phase Shift (degree)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -102,7 +65,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -110,49 +73,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -211,15 +143,33 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
+  <c:style val="2"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -228,26 +178,26 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:defRPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
@@ -261,8 +211,9 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="line"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -279,9 +230,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
                 <a:srgbClr val="004586"/>
@@ -293,13 +241,26 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
             <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:yVal>
             <c:numRef>
@@ -311,7 +272,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>49</c:v>
@@ -323,7 +284,7 @@
                   <c:v>5.28</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.56</c:v>
+                  <c:v>4.5599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1.28</c:v>
@@ -332,7 +293,7 @@
                   <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.074</c:v>
+                  <c:v>7.3999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.5</c:v>
@@ -341,7 +302,20 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7B09-4DA3-B0AF-CDE66691D54D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:axId val="56848390"/>
         <c:axId val="53101642"/>
       </c:scatterChart>
@@ -360,26 +334,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
@@ -398,26 +372,28 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="53101642"/>
@@ -435,7 +411,7 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -447,26 +423,26 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:defRPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
-                        <a:srgbClr val="ffffff"/>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                     </a:uFill>
                     <a:latin typeface="Arial"/>
@@ -485,26 +461,28 @@
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:txPr>
           <a:bodyPr/>
+          <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:uFill>
                   <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
+                    <a:srgbClr val="FFFFFF"/>
                   </a:solidFill>
                 </a:uFill>
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="56848390"/>
@@ -515,7 +493,7 @@
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -532,20 +510,26 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="span"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -559,14 +543,14 @@
       <xdr:row>32</xdr:row>
       <xdr:rowOff>28440</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20160" y="2016000"/>
-        <a:ext cx="5670360" cy="3234600"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -579,23 +563,279 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col min="1" max="1025" width="11.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,229 +855,228 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>0.1</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" s="1">
         <v>25000</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="1">
         <v>90</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>30</v>
       </c>
-      <c r="C3" s="1" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <f aca="false">(1/B3)</f>
-        <v>0.0333333333333333</v>
-      </c>
-      <c r="E3" s="1" t="n">
+      <c r="C3" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D11" si="0">(1/B3)</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E3" s="1">
         <v>9000</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <f aca="false">(360*B3*(E3*10^-6))</f>
-        <v>97.2</v>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F11" si="1">(360*B3*(E3*10^-6))</f>
+        <v>97.199999999999989</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>100</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="1">
         <v>49</v>
       </c>
-      <c r="D4" s="1" t="n">
-        <f aca="false">(1/B4)</f>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="1">
         <v>2480</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <f aca="false">(360*B4*(E4*10^-6))</f>
+      <c r="F4" s="1">
+        <f t="shared" si="1"/>
         <v>89.28</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>300</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="1">
         <v>1.4</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <f aca="false">(1/B5)</f>
-        <v>0.00333333333333333</v>
-      </c>
-      <c r="E5" s="1" t="n">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="E5" s="1">
         <v>760</v>
       </c>
-      <c r="F5" s="1" t="n">
-        <f aca="false">(360*B5*(E5*10^-6))</f>
+      <c r="F5" s="1">
+        <f t="shared" si="1"/>
         <v>82.08</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="1">
         <v>1000</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="1">
         <v>5.28</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <f aca="false">(1/B6)</f>
-        <v>0.001</v>
-      </c>
-      <c r="E6" s="1" t="n">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>1E-3</v>
+      </c>
+      <c r="E6" s="1">
         <v>116</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <f aca="false">(360*B6*(E6*10^-6))</f>
+      <c r="F6" s="1">
+        <f t="shared" si="1"/>
         <v>41.76</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="1">
         <v>3000</v>
       </c>
-      <c r="C7" s="1" t="n">
-        <v>4.56</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <f aca="false">(1/B7)</f>
-        <v>0.000333333333333333</v>
-      </c>
-      <c r="E7" s="1" t="n">
+      <c r="C7" s="1">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333332E-4</v>
+      </c>
+      <c r="E7" s="1">
         <v>46</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <f aca="false">(360*B7*(E7*10^-6))</f>
+      <c r="F7" s="1">
+        <f t="shared" si="1"/>
         <v>49.68</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>10000</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="1">
         <v>1.28</v>
       </c>
-      <c r="D8" s="1" t="n">
-        <f aca="false">(1/B8)</f>
-        <v>0.0001</v>
-      </c>
-      <c r="E8" s="1" t="n">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>1E-4</v>
+      </c>
+      <c r="E8" s="1">
         <v>23</v>
       </c>
-      <c r="F8" s="1" t="n">
-        <f aca="false">(360*B8*(E8*10^-6))</f>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
         <v>82.8</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" s="1">
         <v>30000</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="1">
         <v>0.4</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <f aca="false">(1/B9)</f>
-        <v>3.33333333333333E-005</v>
-      </c>
-      <c r="E9" s="1" t="n">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335E-5</v>
+      </c>
+      <c r="E9" s="1">
         <v>8.6</v>
       </c>
-      <c r="F9" s="1" t="n">
-        <f aca="false">(360*B9*(E9*10^-6))</f>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
         <v>92.88</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" s="1">
         <v>100000</v>
       </c>
-      <c r="C10" s="1" t="n">
-        <v>0.074</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <f aca="false">(1/B10)</f>
-        <v>1E-005</v>
-      </c>
-      <c r="E10" s="1" t="n">
+      <c r="C10" s="1">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="E10" s="1">
         <v>2.4</v>
       </c>
-      <c r="F10" s="1" t="n">
-        <f aca="false">(360*B10*(E10*10^-6))</f>
-        <v>86.4</v>
+      <c r="F10" s="1">
+        <f t="shared" si="1"/>
+        <v>86.399999999999991</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>300000</v>
       </c>
-      <c r="C11" s="1" t="n">
+      <c r="C11" s="1">
         <v>0.5</v>
       </c>
-      <c r="D11" s="1" t="n">
-        <f aca="false">(1/B11)</f>
-        <v>3.33333333333333E-006</v>
-      </c>
-      <c r="E11" s="1" t="n">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333333E-6</v>
+      </c>
+      <c r="E11" s="1">
         <v>0.92</v>
       </c>
-      <c r="F11" s="1" t="n">
-        <f aca="false">(360*B11*(E11*10^-6))</f>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
         <v>99.36</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>